<commit_message>
18:12 time 25.03.2024 day
</commit_message>
<xml_diff>
--- a/file_service/person.xlsx
+++ b/file_service/person.xlsx
@@ -522,72 +522,72 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>40</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>40</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>39</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>42</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>41</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>41</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>41</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>39</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>41</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>40</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>42</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>540</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>475</t>
         </is>
       </c>
     </row>
@@ -599,72 +599,72 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>19</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>22</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>19</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>19</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>19</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>300</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>173</t>
+          <t>229</t>
         </is>
       </c>
     </row>

</xml_diff>